<commit_message>
Se crea modelo de base de datos, script de creación y diagrama relacional
</commit_message>
<xml_diff>
--- a/baseDeDatos/Modelo BD.xlsx
+++ b/baseDeDatos/Modelo BD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmontoya\desarrollo\makaia\proyecto\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmontoya\desarrollo\makaia\proyecto\baseDeDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC87738-1D72-4753-BA34-84C397BBDDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7EA760-D2D6-467F-9BDA-14C112C1C7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FC0B5289-ED1D-4648-B595-1FE32A83BF5D}"/>
   </bookViews>
@@ -263,6 +263,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -270,9 +273,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA776EE-7F6C-4130-9885-54D0709BC929}">
   <dimension ref="A2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -617,24 +617,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="6"/>
+      <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -669,21 +669,21 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -721,23 +721,23 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="F10" s="6" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -782,14 +782,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:N10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>